<commit_message>
pedemeia33 - modelos probit evasão (1.4_Probit.R) finalizados - windows 24012025
</commit_message>
<xml_diff>
--- a/Codigo Novo pdm/Script pdm/Docs Acessorios pdm/Tabela Variaveis Analises Pe de Meia.xlsx
+++ b/Codigo Novo pdm/Script pdm/Docs Acessorios pdm/Tabela Variaveis Analises Pe de Meia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/1. Educacao/2. Academia/3. DOUTORADO/USP - Economia Aplicada/MATERIAS/Eco II - Daniel/Desafio Eco II - Pe de Meia/Github/pedemeia24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/1. Educacao/2. Academia/3. DOUTORADO/USP - Economia Aplicada/MATERIAS/Eco II - Daniel/Desafio Eco II - Pe de Meia/Github/pedemeia33/Codigo Novo pdm/Script pdm/Docs Acessorios pdm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{F1CD36D2-19BE-47EB-AE65-13017DD7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB632AA6-E7BE-4EDE-932C-0BA0B1556FC9}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{F1CD36D2-19BE-47EB-AE65-13017DD7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A29536E8-E832-4182-9343-A98288512382}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F24F635-5B38-4FE0-8A30-7E7C7EEBC13B}"/>
   </bookViews>
@@ -1590,10 +1590,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247AA1CF-A420-4D91-B350-1F036DB135E9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,7 +1634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2050,7 +2051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2284,7 +2285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2362,7 +2363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2519,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>6</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
@@ -2623,7 +2624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
@@ -2701,7 +2702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>12</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>13</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>14</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>15</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>16</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>17</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>18</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>19</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>20</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>21</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>22</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>23</v>
       </c>
@@ -3039,7 +3040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>24</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>25</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>26</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>27</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>28</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>29</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>30</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>31</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>32</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>33</v>
       </c>
@@ -3299,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>34</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="10">
         <v>35</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1</v>
       </c>
@@ -3377,7 +3378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3</v>
       </c>
@@ -3431,7 +3432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4</v>
       </c>
@@ -3458,7 +3459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>5</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>6</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>7</v>
       </c>
@@ -3539,7 +3540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>8</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>9</v>
       </c>
@@ -3593,7 +3594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>10</v>
       </c>
@@ -3620,7 +3621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>11</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>12</v>
       </c>
@@ -3674,7 +3675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>13</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>14</v>
       </c>
@@ -3728,7 +3729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>15</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>16</v>
       </c>
@@ -3782,7 +3783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>17</v>
       </c>
@@ -3809,7 +3810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="10">
         <v>18</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1</v>
       </c>
@@ -3855,7 +3856,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2</v>
       </c>
@@ -3874,7 +3875,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>3</v>
       </c>
@@ -3893,7 +3894,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -3912,7 +3913,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>5</v>
       </c>
@@ -3931,7 +3932,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>6</v>
       </c>
@@ -3950,7 +3951,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>7</v>
       </c>
@@ -3969,7 +3970,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>8</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>9</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>10</v>
       </c>
@@ -4026,7 +4027,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>11</v>
       </c>
@@ -4045,7 +4046,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>12</v>
       </c>
@@ -4064,7 +4065,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>13</v>
       </c>
@@ -4083,7 +4084,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>14</v>
       </c>
@@ -4102,7 +4103,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>15</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>16</v>
       </c>
@@ -4140,7 +4141,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>17</v>
       </c>
@@ -4159,7 +4160,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>18</v>
       </c>
@@ -4178,7 +4179,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>19</v>
       </c>
@@ -4197,7 +4198,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>20</v>
       </c>
@@ -4216,7 +4217,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>21</v>
       </c>
@@ -4235,7 +4236,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>22</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>23</v>
       </c>
@@ -4273,7 +4274,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>24</v>
       </c>
@@ -4292,7 +4293,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>25</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>26</v>
       </c>
@@ -4330,7 +4331,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>27</v>
       </c>
@@ -4349,7 +4350,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>28</v>
       </c>
@@ -4368,7 +4369,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>29</v>
       </c>
@@ -4387,7 +4388,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>30</v>
       </c>
@@ -4406,7 +4407,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>31</v>
       </c>
@@ -4425,7 +4426,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>32</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>33</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>34</v>
       </c>
@@ -4482,7 +4483,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>35</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>36</v>
       </c>
@@ -4520,7 +4521,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>37</v>
       </c>
@@ -4539,7 +4540,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>38</v>
       </c>
@@ -4558,7 +4559,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>39</v>
       </c>
@@ -4577,7 +4578,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>40</v>
       </c>
@@ -4596,7 +4597,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>41</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>42</v>
       </c>
@@ -4634,7 +4635,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>43</v>
       </c>
@@ -4653,7 +4654,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>44</v>
       </c>
@@ -4672,7 +4673,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="10" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" s="10" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="10">
         <v>45</v>
       </c>
@@ -4693,7 +4694,7 @@
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1</v>
       </c>
@@ -4711,7 +4712,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2</v>
       </c>
@@ -4729,7 +4730,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>3</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>4</v>
       </c>
@@ -4765,7 +4766,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>5</v>
       </c>
@@ -4783,7 +4784,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>6</v>
       </c>
@@ -4801,7 +4802,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>7</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>8</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>9</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>10</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>11</v>
       </c>
@@ -4891,7 +4892,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>12</v>
       </c>
@@ -4909,7 +4910,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>13</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>14</v>
       </c>
@@ -4945,7 +4946,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>15</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>16</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>17</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>18</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>19</v>
       </c>
@@ -5035,7 +5036,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>20</v>
       </c>
@@ -5053,7 +5054,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>21</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>22</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>23</v>
       </c>
@@ -5107,7 +5108,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>24</v>
       </c>
@@ -5125,7 +5126,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>25</v>
       </c>
@@ -5143,7 +5144,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>26</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>27</v>
       </c>
@@ -5179,7 +5180,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>28</v>
       </c>
@@ -5197,7 +5198,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>29</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>30</v>
       </c>
@@ -5233,7 +5234,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>31</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>32</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>33</v>
       </c>
@@ -5287,7 +5288,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="10">
         <v>34</v>
       </c>
@@ -5307,7 +5308,7 @@
       <c r="G164" s="12"/>
       <c r="H164" s="12"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>1</v>
       </c>
@@ -5333,7 +5334,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>2</v>
       </c>
@@ -5359,7 +5360,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>3</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>4</v>
       </c>
@@ -5411,7 +5412,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>5</v>
       </c>
@@ -5437,7 +5438,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>6</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>7</v>
       </c>
@@ -5489,7 +5490,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>8</v>
       </c>
@@ -5515,7 +5516,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>9</v>
       </c>
@@ -5541,7 +5542,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>10</v>
       </c>
@@ -5567,7 +5568,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>11</v>
       </c>
@@ -5593,7 +5594,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>12</v>
       </c>
@@ -5619,7 +5620,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>13</v>
       </c>
@@ -5645,7 +5646,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>14</v>
       </c>
@@ -5671,7 +5672,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>15</v>
       </c>
@@ -5697,7 +5698,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>16</v>
       </c>
@@ -5723,7 +5724,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>17</v>
       </c>
@@ -5749,7 +5750,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>18</v>
       </c>
@@ -5775,7 +5776,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>19</v>
       </c>
@@ -5801,7 +5802,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>20</v>
       </c>
@@ -5827,7 +5828,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>21</v>
       </c>
@@ -5879,7 +5880,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>23</v>
       </c>
@@ -5905,7 +5906,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>24</v>
       </c>
@@ -5931,7 +5932,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>25</v>
       </c>
@@ -5957,7 +5958,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>26</v>
       </c>
@@ -5983,7 +5984,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>27</v>
       </c>
@@ -6009,7 +6010,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>28</v>
       </c>
@@ -6035,7 +6036,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>29</v>
       </c>
@@ -6061,7 +6062,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>30</v>
       </c>
@@ -6087,7 +6088,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>31</v>
       </c>
@@ -6113,7 +6114,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>32</v>
       </c>
@@ -6139,7 +6140,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>33</v>
       </c>
@@ -6165,7 +6166,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>34</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>35</v>
       </c>
@@ -6217,7 +6218,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>36</v>
       </c>
@@ -6243,7 +6244,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>37</v>
       </c>
@@ -6269,7 +6270,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>38</v>
       </c>
@@ -6295,7 +6296,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>39</v>
       </c>
@@ -6322,6 +6323,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H203" xr:uid="{247AA1CF-A420-4D91-B350-1F036DB135E9}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="VD3004"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>